<commit_message>
Starting FrontEnd, some minor improvements, Improving scoring section
</commit_message>
<xml_diff>
--- a/dq/template/usecase_template.xlsx
+++ b/dq/template/usecase_template.xlsx
@@ -23,6 +23,21 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="181">
   <si>
+    <t xml:space="preserve">Note that existing use case FFP profiles are listed in usecase/usecase_definition.xlsx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to use this template: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in the second "Use case template" tab in this spreadsheet to add new use case FFP profiles and FFP assertions representing their possible categories. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a) The desired name for one or more FFP use case profile (and its category) should be entered in cell B1 onwards (i.e. C1, D1, E1, etc.). Refer to existing use case FFP profiles for examples. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(b) For each FFP use case profile's category (i.e. column), enter "1" to indicate which FFP assertion/s are relevant to that column. </t>
+  </si>
+  <si>
     <t>Data Quality Assertion</t>
   </si>
   <si>
@@ -549,21 +564,6 @@
   </si>
   <si>
     <t>If the datum link reference in the 'geo:hasGeometry' field does not correspond to any of the specified types (AGD84, GDA2020, GDA94, WGS84), label the record as 'None'. This label indicates that the datum used does not match the predefined types, suggesting either a different standard is in use or the datum type is unspecified.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note that existing use case FFP profiles are listed in usecase/usecase_definition.xlsx </t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to use this template: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(a) The desired name for one or more FFP use case profile (and its category) should be entered in cell B1 onwards (i.e. C1, D1, E1, etc.). Refer to existing use case FFP profiles for examples. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(b) For each FFP use case profile's category (i.e. column), enter "1" to indicate which FFP assertion/s are relevant to that column. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fill in the second "Use case template" tab in this spreadsheet to add new use case FFP profiles and FFP assertions representing their possible categories. </t>
   </si>
 </sst>
 </file>
@@ -579,11 +579,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF0D0D0D"/>
       <name val="Segoe UI"/>
@@ -595,6 +590,11 @@
       <color rgb="FF0D0D0D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -634,11 +634,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,37 +949,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="180.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="180.73046875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A1" s="2" t="s">
-        <v>176</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A3" s="3" t="s">
-        <v>177</v>
+      <c r="A3" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A4" s="2" t="s">
-        <v>180</v>
+      <c r="A4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A5" s="2" t="s">
-        <v>178</v>
+      <c r="A5" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A6" s="2" t="s">
-        <v>179</v>
+      <c r="A6" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -988,7 +988,7 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -998,226 +998,226 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1230,7 +1230,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1244,883 +1244,883 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D23" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E23" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F23" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E24" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F24" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E25" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="F27" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E28" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F29" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D30" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E30" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F30" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E31" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E32" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F32" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D33" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F33" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="F34" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C35" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="F35" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E36" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="F36" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E37" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F37" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E38" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="F38" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E39" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F39" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F40" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D41" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F41" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E42" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F42" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E43" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="F43" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D44" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E44" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="F44" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting Visualization and some more improvements
</commit_message>
<xml_diff>
--- a/dq/template/usecase_template.xlsx
+++ b/dq/template/usecase_template.xlsx
@@ -522,7 +522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -753,7 +753,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>date_format_validation:valid</t>
+          <t>duplicate_value_combination:inferred_duplicate</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -761,7 +761,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>date_format_validation:invalid</t>
+          <t>duplicate_value_combination:inferred_nonduplicate</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -769,7 +769,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>date_completeness:empty</t>
+          <t>geo_spatial_accuracy_precision:low_precision</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -777,7 +777,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>date_completeness:non_empty</t>
+          <t>geo_spatial_accuracy_precision:high_precision</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -785,7 +785,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>date_outlier_kmeans:outlier_date</t>
+          <t>date_format_validation:valid</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -793,7 +793,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>date_outlier_kmeans:normal_date</t>
+          <t>date_format_validation:invalid</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -801,7 +801,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>date_outlier_irq:outlier_date</t>
+          <t>date_completeness:empty</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -809,7 +809,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>date_outlier_irq:normal_date</t>
+          <t>date_completeness:non_empty</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -817,7 +817,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>scientific_name_completeness:empty_name</t>
+          <t>date_outlier_kmeans:outlier_date</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -825,7 +825,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>scientific_name_completeness:non_empty_name</t>
+          <t>date_outlier_kmeans:normal_date</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -833,7 +833,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>scientific_name_validation:valid_name</t>
+          <t>date_outlier_irq:outlier_date</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -841,7 +841,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>scientific_name_validation:invalid_name</t>
+          <t>date_outlier_irq:normal_date</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -849,7 +849,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>datum_completeness:empty</t>
+          <t>scientific_name_completeness:empty_name</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -857,7 +857,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>datum_completeness:not_empty</t>
+          <t>scientific_name_completeness:non_empty_name</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -865,7 +865,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>datum_validation:valid</t>
+          <t>scientific_name_validation:valid_name</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -873,7 +873,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>datum_validation:invalid</t>
+          <t>scientific_name_validation:invalid_name</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -881,7 +881,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>datum_type:AGD84</t>
+          <t>datum_completeness:empty</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -889,7 +889,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>datum_type:GDA2020</t>
+          <t>datum_completeness:not_empty</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -897,7 +897,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>datum_type:GDA94</t>
+          <t>datum_validation:valid</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -905,7 +905,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>datum_type:WGS84</t>
+          <t>datum_validation:invalid</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -913,10 +913,42 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>datum_type:AGD84</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>datum_type:GDA2020</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>datum_type:GDA94</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>datum_type:WGS84</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>datum_type:None</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -929,7 +961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1804,135 +1836,135 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>date_format_validation:valid</t>
+          <t>duplicate_value_combination:inferred_duplicate</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>data_quality</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>sosa:phenomenonTime</t>
+          <t>various_fields</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>valid</t>
+          <t>inferred_duplicate</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Indicates that the date format is valid and recognized.</t>
+          <t>Indicates that the record has a combination of values across multiple fields that are identical to other records.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t xml:space="preserve">If the date format in the 'sosa:phenomenonTime' field adheres to recognized and accepted standards, label the record as 'valid'. This indicates that the date is structured in a manner that is universally understood and correctly interpretable by systems and users alike. </t>
+          <t>If the record has a combination of values across the specified fields that is identical to other records in the dataset, label it as 'duplicate_combination'. This implies redundancy in data values for multiple records.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>date_format_validation:invalid</t>
+          <t>duplicate_value_combination:inferred_nonduplicate</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>data_quality</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>sosa:phenomenonTime</t>
+          <t>various_fields</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>invalid</t>
+          <t>inferred_nonduplicate</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Indicates that the date format is invalid or unrecognized.</t>
+          <t>Indicates that the record has a unique combination of values across multiple fields that is not shared by other records.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>If the date format in the 'sosa:phenomenonTime' field does not follow recognized and accepted standards or is structured in a way that is not correctly interpretable (e.g., mixing up day and month in a non-standard format), label the record as 'invalid'. This suggests that the date may be prone to misinterpretation or errors in processing due to its unconventional format.</t>
+          <t>If the record has a unique combination of values across the specified fields, label it as 'unique_combination'. This means that no other records share this exact combination.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>date_completeness:empty</t>
+          <t>geo_spatial_accuracy_precision:low_precision</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>geo</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>sosa:phenomenonTime</t>
+          <t>geo:hasMetricSpatialAccuracy</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>empty</t>
+          <t>low_precision</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Indicates that the date is empty.</t>
+          <t>Indicates that the spatial accuracy is low, either because the value of coordinateUncertaintyInMeters is empty or exceeds 10,000 meters.</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>If the 'sosa:phenomenonTime' field does not exist or contains no data for a given record, label the record as 'empty'. This indicates that there is no date information provided, signifying an absence of temporal data for the observation. Non_Empty: If the 'sosa:phenomenonTime' field exists and contains data for a given record, label the record as 'non_empty'. This signifies that date information is present, indicating the availability of temporal data for the observation.</t>
+          <t>If the 'coordinateUncertaintyInMeters' field is empty or its value exceeds 10,000, label the record as 'low_precision'. This indicates that the precision of the spatial accuracy is insufficient.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>date_completeness:non_empty</t>
+          <t>geo_spatial_accuracy_precision:high_precision</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>geo</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>sosa:phenomenonTime</t>
+          <t>geo:hasMetricSpatialAccuracy</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>non_empty</t>
+          <t>high_precision</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Indicates that the date is not empty.</t>
+          <t>Indicates that the spatial accuracy is high, meaning the value of coordinateUncertaintyInMeters is less than or equal to 10,000 meters.</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>If the 'sosa:phenomenonTime' field does not exist or contains no data for a given record, label the record as 'empty'. This indicates that there is no date information provided, signifying an absence of temporal data for the observation. Non_Empty: If the 'sosa:phenomenonTime' field exists and contains data for a given record, label the record as 'non_empty'. This signifies that date information is present, indicating the availability of temporal data for the observation.</t>
+          <t>If the 'coordinateUncertaintyInMeters' field contains a value of 10,000 or less, label the record as 'high_precision'. This indicates that the precision of the spatial accuracy is adequate.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>date_outlier_kmeans:outlier_date</t>
+          <t>date_format_validation:valid</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1947,24 +1979,24 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>outlier_date</t>
+          <t>valid</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>This label is used to tag dates that are determined to be significantly different from the majority, based on the KMeans clustering algorithm. Such dates fall into the smallest cluster or are far from the centroids of their clusters, indicating they deviate notably from typical date values.</t>
+          <t>Indicates that the date format is valid and recognized.</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t xml:space="preserve">If the date from the 'sosa:phenomenonTime' field is significantly different from the majority, as determined by falling into the smallest cluster or being far from the centroids of their clusters when analyzed by the KMeans clustering algorithm, label the record as 'outlier_date'. This label indicates the date deviates notably from typical date values, suggesting it might be an outlier. </t>
+          <t xml:space="preserve">If the date format in the 'sosa:phenomenonTime' field adheres to recognized and accepted standards, label the record as 'valid'. This indicates that the date is structured in a manner that is universally understood and correctly interpretable by systems and users alike. </t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>date_outlier_kmeans:normal_date</t>
+          <t>date_format_validation:invalid</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1979,24 +2011,24 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>normal_date</t>
+          <t>invalid</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>This label is applied to dates that are considered to be within the expected range, based on the KMeans clustering results. These dates fall into larger clusters and are close to the centroids, indicating they align with the common patterns observed in the dataset.</t>
+          <t>Indicates that the date format is invalid or unrecognized.</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>If the date from the 'sosa:phenomenonTime' field falls into larger clusters and is close to the centroids, according to the KMeans clustering results, label the record as 'normal_date'. This suggests the date aligns with common patterns observed in the dataset, indicating it is within the expected range of dates and considered normal.</t>
+          <t>If the date format in the 'sosa:phenomenonTime' field does not follow recognized and accepted standards or is structured in a way that is not correctly interpretable (e.g., mixing up day and month in a non-standard format), label the record as 'invalid'. This suggests that the date may be prone to misinterpretation or errors in processing due to its unconventional format.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>date_outlier_irq:outlier_date</t>
+          <t>date_completeness:empty</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2011,24 +2043,24 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>outlier_date</t>
+          <t>empty</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>This label indicates that the observation date significantly deviates from the typical range, suggesting it may be an anomaly. (Based on IRQ Method)</t>
+          <t>Indicates that the date is empty.</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>If the date from the 'sosa:phenomenonTime' field significantly deviates from the typical range, based on the Interquartile Range (IRQ) method—meaning it falls outside the bounds established by the IRQ calculations (e.g., below Q1 - 1.5IQR or above Q3 + 1.5IQR)—label the record as 'outlier_date'. This label indicates that the date is considered an anomaly, deviating notably from the expected date range.</t>
+          <t>If the 'sosa:phenomenonTime' field does not exist or contains no data for a given record, label the record as 'empty'. This indicates that there is no date information provided, signifying an absence of temporal data for the observation. Non_Empty: If the 'sosa:phenomenonTime' field exists and contains data for a given record, label the record as 'non_empty'. This signifies that date information is present, indicating the availability of temporal data for the observation.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>date_outlier_irq:normal_date</t>
+          <t>date_completeness:non_empty</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2043,280 +2075,280 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>normal_date</t>
+          <t>non_empty</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>This label indicates that the observation date falls within the typical range, suggesting it is not an anomaly. (Based on IRQ Method)</t>
+          <t>Indicates that the date is not empty.</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>If the date from the 'sosa:phenomenonTime' field falls within the typical range, as determined by the Interquartile Range (IRQ) method—meaning it is within the bounds set by Q1 - 1.5IQR and Q3 + 1.5IQR—label the record as 'normal_date'. This suggests the date does not significantly deviate from what is typically observed, indicating it is not considered an anomaly.</t>
+          <t>If the 'sosa:phenomenonTime' field does not exist or contains no data for a given record, label the record as 'empty'. This indicates that there is no date information provided, signifying an absence of temporal data for the observation. Non_Empty: If the 'sosa:phenomenonTime' field exists and contains data for a given record, label the record as 'non_empty'. This signifies that date information is present, indicating the availability of temporal data for the observation.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>scientific_name_completeness:empty_name</t>
+          <t>date_outlier_kmeans:outlier_date</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>scientific_name</t>
+          <t>date</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>tern:FeatureOfInterest</t>
+          <t>sosa:phenomenonTime</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>empty_name</t>
+          <t>outlier_date</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>This label is used to mark records where the scientific name field is missing or contains no data, indicating a lack of specified scientific identification for the observation or entity.</t>
+          <t>This label is used to tag dates that are determined to be significantly different from the majority, based on the KMeans clustering algorithm. Such dates fall into the smallest cluster or are far from the centroids of their clusters, indicating they deviate notably from typical date values.</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t xml:space="preserve">If the 'tern:FeatureOfInterest' field does not exist or contains no data for a given record, label the record as 'empty_name'. This indicates the absence of a scientific name, signifying that specific scientific identification for the observation or entity is missing. </t>
+          <t xml:space="preserve">If the date from the 'sosa:phenomenonTime' field is significantly different from the majority, as determined by falling into the smallest cluster or being far from the centroids of their clusters when analyzed by the KMeans clustering algorithm, label the record as 'outlier_date'. This label indicates the date deviates notably from typical date values, suggesting it might be an outlier. </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>scientific_name_completeness:non_empty_name</t>
+          <t>date_outlier_kmeans:normal_date</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>scientific_name</t>
+          <t>date</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>tern:FeatureOfInterest</t>
+          <t>sosa:phenomenonTime</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>non_empty_name</t>
+          <t>normal_date</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>This label is applied to records that have a valid scientific name provided, indicating the presence of specified scientific identification for the observation or entity.</t>
+          <t>This label is applied to dates that are considered to be within the expected range, based on the KMeans clustering results. These dates fall into larger clusters and are close to the centroids, indicating they align with the common patterns observed in the dataset.</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>If the 'tern:FeatureOfInterest' field exists and contains data for a given record, label the record as 'non_empty_name'. This signifies the presence of a scientific name, indicating that specific scientific identification for the observation or entity has been provided.</t>
+          <t>If the date from the 'sosa:phenomenonTime' field falls into larger clusters and is close to the centroids, according to the KMeans clustering results, label the record as 'normal_date'. This suggests the date aligns with common patterns observed in the dataset, indicating it is within the expected range of dates and considered normal.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>scientific_name_validation:valid_name</t>
+          <t>date_outlier_irq:outlier_date</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>scientific_name</t>
+          <t>date</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>tern:FeatureOfInterest</t>
+          <t>sosa:phenomenonTime</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>valid_name</t>
+          <t>outlier_date</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>This label is applied to records where the scientific name has been verified as correct and adheres to accepted naming conventions or validation criteria, indicating the scientific name is legitimate and accurately represents the entity.</t>
+          <t>This label indicates that the observation date significantly deviates from the typical range, suggesting it may be an anomaly. (Based on IRQ Method)</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t xml:space="preserve">If the scientific name in the 'tern:FeatureOfInterest' field has been verified against accepted naming conventions or validation criteria and is found to be correct, label the record as 'valid_name'. This indicates that the scientific name is legitimate and accurately represents the observed entity, adhering to the recognized standards for scientific nomenclature. </t>
+          <t>If the date from the 'sosa:phenomenonTime' field significantly deviates from the typical range, based on the Interquartile Range (IRQ) method—meaning it falls outside the bounds established by the IRQ calculations (e.g., below Q1 - 1.5IQR or above Q3 + 1.5IQR)—label the record as 'outlier_date'. This label indicates that the date is considered an anomaly, deviating notably from the expected date range.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>scientific_name_validation:invalid_name</t>
+          <t>date_outlier_irq:normal_date</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>scientific_name</t>
+          <t>date</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>tern:FeatureOfInterest</t>
+          <t>sosa:phenomenonTime</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>invalid_name</t>
+          <t>normal_date</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>This label is used for records with scientific names that do not meet the established validation criteria, suggesting the name might be incorrect, misspelled, or not conforming to accepted scientific naming conventions.</t>
+          <t>This label indicates that the observation date falls within the typical range, suggesting it is not an anomaly. (Based on IRQ Method)</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>If the scientific name in the 'tern:FeatureOfInterest' field does not meet established validation criteria—whether due to being incorrect, misspelled, or not conforming to accepted scientific naming conventions—label the record as 'invalid_name'. This suggests that the name may not be legitimate or accurately represent the entity as per the recognized standards for scientific nomenclature.</t>
+          <t>If the date from the 'sosa:phenomenonTime' field falls within the typical range, as determined by the Interquartile Range (IRQ) method—meaning it is within the bounds set by Q1 - 1.5IQR and Q3 + 1.5IQR—label the record as 'normal_date'. This suggests the date does not significantly deviate from what is typically observed, indicating it is not considered an anomaly.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>datum_completeness:empty</t>
+          <t>scientific_name_completeness:empty_name</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>datum</t>
+          <t>scientific_name</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>geo:hasGeometry</t>
+          <t>tern:FeatureOfInterest</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>empty</t>
+          <t>empty_name</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Indicates that the datum link reference is empty.</t>
+          <t>This label is used to mark records where the scientific name field is missing or contains no data, indicating a lack of specified scientific identification for the observation or entity.</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t xml:space="preserve">If the 'geo:hasGeometry' field either does not exist or contains no link reference data for a given record, label the record as 'empty'. This label indicates the absence of a datum link reference, signifying that no specific geographic datum information is provided for the geographic coordinate data. </t>
+          <t xml:space="preserve">If the 'tern:FeatureOfInterest' field does not exist or contains no data for a given record, label the record as 'empty_name'. This indicates the absence of a scientific name, signifying that specific scientific identification for the observation or entity is missing. </t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>datum_completeness:not_empty</t>
+          <t>scientific_name_completeness:non_empty_name</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>datum</t>
+          <t>scientific_name</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>geo:hasGeometry</t>
+          <t>tern:FeatureOfInterest</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>not_empty</t>
+          <t>non_empty_name</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Indicates that the datum link reference is not empty.</t>
+          <t>This label is applied to records that have a valid scientific name provided, indicating the presence of specified scientific identification for the observation or entity.</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>If the 'geo:hasGeometry' field exists and contains link reference data for a given record, label the record as 'not_empty'. This label signifies the presence of a datum link reference, indicating that specific geographic datum information is provided for the geographic coordinate data.</t>
+          <t>If the 'tern:FeatureOfInterest' field exists and contains data for a given record, label the record as 'non_empty_name'. This signifies the presence of a scientific name, indicating that specific scientific identification for the observation or entity has been provided.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>datum_validation:valid</t>
+          <t>scientific_name_validation:valid_name</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>datum</t>
+          <t>scientific_name</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>geo:hasGeometry</t>
+          <t>tern:FeatureOfInterest</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>valid</t>
+          <t>valid_name</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Indicates that the datum link reference is valid and recognized.</t>
+          <t>This label is applied to records where the scientific name has been verified as correct and adheres to accepted naming conventions or validation criteria, indicating the scientific name is legitimate and accurately represents the entity.</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>If the datum link reference in the 'geo:hasGeometry' field is recognized and conforms to known and accepted geographic datum standards, label the record as 'valid'. This indicates that the datum link reference is appropriate and can be reliably used for geographic coordinate data interpretation.</t>
+          <t xml:space="preserve">If the scientific name in the 'tern:FeatureOfInterest' field has been verified against accepted naming conventions or validation criteria and is found to be correct, label the record as 'valid_name'. This indicates that the scientific name is legitimate and accurately represents the observed entity, adhering to the recognized standards for scientific nomenclature. </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>datum_validation:invalid</t>
+          <t>scientific_name_validation:invalid_name</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>datum</t>
+          <t>scientific_name</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>geo:hasGeometry</t>
+          <t>tern:FeatureOfInterest</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>invalid</t>
+          <t>invalid_name</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Indicates that the datum link reference is invalid or unrecognized.</t>
+          <t>This label is used for records with scientific names that do not meet the established validation criteria, suggesting the name might be incorrect, misspelled, or not conforming to accepted scientific naming conventions.</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>If the datum link reference in the 'geo:hasGeometry' field is not recognized or does not conform to known and accepted geographic datum standards, label the record as 'invalid'. This indicates that the datum link reference may be incorrect, fabricated, or not suitable for accurate geographic coordinate data interpretation.</t>
+          <t>If the scientific name in the 'tern:FeatureOfInterest' field does not meet established validation criteria—whether due to being incorrect, misspelled, or not conforming to accepted scientific naming conventions—label the record as 'invalid_name'. This suggests that the name may not be legitimate or accurately represent the entity as per the recognized standards for scientific nomenclature.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>datum_type:AGD84</t>
+          <t>datum_completeness:empty</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2331,24 +2363,24 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>AGD84</t>
+          <t>empty</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Indicates that the datum is in the Australian Geodetic Datum 1984 type.</t>
+          <t>Indicates that the datum link reference is empty.</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t xml:space="preserve">If the datum link reference within the 'geo:hasGeometry' field specifies the Australian Geodetic Datum 1984 (AGD84), label the record as 'AGD84'. This classification indicates that the geographic data is referenced according to the AGD84 standard. </t>
+          <t xml:space="preserve">If the 'geo:hasGeometry' field either does not exist or contains no link reference data for a given record, label the record as 'empty'. This label indicates the absence of a datum link reference, signifying that no specific geographic datum information is provided for the geographic coordinate data. </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>datum_type:GDA2020</t>
+          <t>datum_completeness:not_empty</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2363,24 +2395,24 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>GDA2020</t>
+          <t>not_empty</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Indicates that the datum is in the Geocentric Datum of Australia 2020 type.</t>
+          <t>Indicates that the datum link reference is not empty.</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t xml:space="preserve">If the datum link reference in the 'geo:hasGeometry' field is identified as the Geocentric Datum of Australia 2020 (GDA2020), label the record as 'GDA2020'. This shows that the geographic data adheres to the GDA2020 standard, a more recent datum for Australia. </t>
+          <t>If the 'geo:hasGeometry' field exists and contains link reference data for a given record, label the record as 'not_empty'. This label signifies the presence of a datum link reference, indicating that specific geographic datum information is provided for the geographic coordinate data.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>datum_type:GDA94</t>
+          <t>datum_validation:valid</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2395,24 +2427,24 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>GDA94</t>
+          <t>valid</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Indicates that the datum is in the Geocentric Datum of Australia 1994 type.</t>
+          <t>Indicates that the datum link reference is valid and recognized.</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>If the datum link reference in the 'geo:hasGeometry' field corresponds to the Geocentric Datum of Australia 1994 (GDA94), label the record as 'GDA94'. This indicates the use of the GDA94 standard, preceding GDA2020 for Australian geographic data.</t>
+          <t>If the datum link reference in the 'geo:hasGeometry' field is recognized and conforms to known and accepted geographic datum standards, label the record as 'valid'. This indicates that the datum link reference is appropriate and can be reliably used for geographic coordinate data interpretation.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>datum_type:WGS84</t>
+          <t>datum_validation:invalid</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2427,47 +2459,175 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>WGS84</t>
+          <t>invalid</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Indicates that the datum is in the World Geodetic System 1984 type.</t>
+          <t>Indicates that the datum link reference is invalid or unrecognized.</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>If the datum link reference in the 'geo:hasGeometry' field is recognized as the World Geodetic System 1984 (WGS84), label the record as 'WGS84'. This classification signifies that the geographic data is based on the globally used WGS84 standard.</t>
+          <t>If the datum link reference in the 'geo:hasGeometry' field is not recognized or does not conform to known and accepted geographic datum standards, label the record as 'invalid'. This indicates that the datum link reference may be incorrect, fabricated, or not suitable for accurate geographic coordinate data interpretation.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>datum_type:AGD84</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>datum</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>geo:hasGeometry</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>AGD84</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Indicates that the datum is in the Australian Geodetic Datum 1984 type.</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If the datum link reference within the 'geo:hasGeometry' field specifies the Australian Geodetic Datum 1984 (AGD84), label the record as 'AGD84'. This classification indicates that the geographic data is referenced according to the AGD84 standard. </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>datum_type:GDA2020</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>datum</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>geo:hasGeometry</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>GDA2020</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Indicates that the datum is in the Geocentric Datum of Australia 2020 type.</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If the datum link reference in the 'geo:hasGeometry' field is identified as the Geocentric Datum of Australia 2020 (GDA2020), label the record as 'GDA2020'. This shows that the geographic data adheres to the GDA2020 standard, a more recent datum for Australia. </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>datum_type:GDA94</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>datum</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>geo:hasGeometry</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>GDA94</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Indicates that the datum is in the Geocentric Datum of Australia 1994 type.</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>If the datum link reference in the 'geo:hasGeometry' field corresponds to the Geocentric Datum of Australia 1994 (GDA94), label the record as 'GDA94'. This indicates the use of the GDA94 standard, preceding GDA2020 for Australian geographic data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>datum_type:WGS84</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>datum</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>geo:hasGeometry</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>WGS84</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Indicates that the datum is in the World Geodetic System 1984 type.</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>If the datum link reference in the 'geo:hasGeometry' field is recognized as the World Geodetic System 1984 (WGS84), label the record as 'WGS84'. This classification signifies that the geographic data is based on the globally used WGS84 standard.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>datum_type:None</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>datum</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>geo:hasGeometry</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>geo:hasGeometry</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>Indicates that the datum is not in the AGD84, GDA2020, GDA94, or WGS84 types.</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>If the datum link reference in the 'geo:hasGeometry' field does not correspond to any of the specified types (AGD84, GDA2020, GDA94, WGS84), label the record as 'None'. This label indicates that the datum used does not match the predefined types, suggesting either a different standard is in use or the datum type is unspecified.</t>
         </is>

</xml_diff>